<commit_message>
- Fixed layout - Fixed descriptions in BOM
</commit_message>
<xml_diff>
--- a/H1DR0/Released/BOM/H1DR01.xlsx
+++ b/H1DR0/Released/BOM/H1DR01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H1DR0x-Hardware\H1DR0\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC80FAE-E9F2-4218-A972-557EC129AE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4503637-269C-4F7E-BB63-5189A39C9D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-1395" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1DR0x" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
-  </si>
-  <si>
     <t xml:space="preserve">TDK </t>
   </si>
   <si>
@@ -232,11 +229,6 @@
     <t>GRM21BC81E475KA12L</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Murata GRM21BC81E475KA12L
-Multilayer Ceramic Capacitor, GRM Series, 4.7 - F, - 10%, X6S, 25 V, 0805 [2012 Metric</t>
-  </si>
-  <si>
     <t>R2, R8, R9</t>
   </si>
   <si>
@@ -328,6 +320,12 @@
   </si>
   <si>
     <t>R3</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 25V X6S 0805</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 30 OHM 0603 1LN</t>
   </si>
 </sst>
 </file>
@@ -969,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1026,7 +1024,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -1043,7 +1041,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1075,19 +1073,19 @@
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="18">
         <v>1</v>
@@ -1095,7 +1093,7 @@
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>17</v>
@@ -1115,19 +1113,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="F11" s="18">
         <v>1</v>
@@ -1135,19 +1133,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F12" s="18">
         <v>3</v>
@@ -1155,19 +1153,19 @@
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F13" s="18">
         <v>1</v>
@@ -1175,19 +1173,19 @@
     </row>
     <row r="14" spans="1:7" ht="56" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" s="18">
         <v>8</v>
@@ -1195,59 +1193,59 @@
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="D15" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="F15" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="F16" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="E17" s="21" t="s">
         <v>23</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>24</v>
       </c>
       <c r="F17" s="18">
         <v>1</v>
@@ -1255,19 +1253,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="D18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="F18" s="18">
         <v>1</v>
@@ -1275,19 +1273,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="C19" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>59</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>60</v>
       </c>
       <c r="F19" s="18">
         <v>1</v>
@@ -1295,19 +1293,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>77</v>
       </c>
       <c r="F20" s="18">
         <v>1</v>
@@ -1315,19 +1313,19 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="D21" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>81</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>83</v>
       </c>
       <c r="F21" s="18">
         <v>1</v>
@@ -1335,19 +1333,19 @@
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
@@ -1355,19 +1353,19 @@
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="E23" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>50</v>
       </c>
       <c r="F23" s="18">
         <v>1</v>
@@ -1375,19 +1373,19 @@
     </row>
     <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="E24" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>93</v>
       </c>
       <c r="F24" s="18">
         <v>1</v>
@@ -1395,19 +1393,19 @@
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="C25" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="18">
         <v>1</v>

</xml_diff>